<commit_message>
small code developments and analyses for SES
</commit_message>
<xml_diff>
--- a/inputData/VencoPy_scalarInputSES.xlsx
+++ b/inputData/VencoPy_scalarInputSES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vencopy_repo\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57B0E4F-BF1F-4217-96AC-02973A6BA686}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDAEA11-05EE-4211-BD64-35B4AF42BF49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,10 +100,10 @@
     <t>Battery capacity</t>
   </si>
   <si>
-    <t>16.04.2020</t>
-  </si>
-  <si>
     <t>Originally from Diego Luca de Tena (DLR-TT) based on the tables from Bernd Propfe (DLR-FK), updated by Niklas Wulff (DLR-TT) as input sheet for VencoPy. Licensed under BSD 3-Clause</t>
+  </si>
+  <si>
+    <t>06.10.2020</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -568,7 +568,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -576,7 +576,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Resolving issue #127 removing all whitespaces from the assumptions excel file
</commit_message>
<xml_diff>
--- a/inputData/VencoPy_scalarInputSES.xlsx
+++ b/inputData/VencoPy_scalarInputSES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vencopy_repo\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDAEA11-05EE-4211-BD64-35B4AF42BF49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACF87F7-9851-4232-A95B-C8C9D23783C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>Minimum daily mileage</t>
-  </si>
-  <si>
     <t>File Info</t>
   </si>
   <si>
@@ -73,37 +70,40 @@
     <t>VencoPy Input Assumptions</t>
   </si>
   <si>
-    <t>Electric consumption NEFZ</t>
-  </si>
-  <si>
-    <t>Fuel consumption NEFZ</t>
-  </si>
-  <si>
-    <t>Electric consumption Artemis</t>
-  </si>
-  <si>
-    <t>Fuel consumption Artemis</t>
-  </si>
-  <si>
-    <t>Maximum SOC</t>
-  </si>
-  <si>
-    <t>Minimum SOC</t>
-  </si>
-  <si>
-    <t>Rated power of charging column</t>
-  </si>
-  <si>
-    <t>Is BEV?</t>
-  </si>
-  <si>
-    <t>Battery capacity</t>
-  </si>
-  <si>
     <t>Originally from Diego Luca de Tena (DLR-TT) based on the tables from Bernd Propfe (DLR-FK), updated by Niklas Wulff (DLR-TT) as input sheet for VencoPy. Licensed under BSD 3-Clause</t>
   </si>
   <si>
     <t>06.10.2020</t>
+  </si>
+  <si>
+    <t>Minimum_daily_mileage</t>
+  </si>
+  <si>
+    <t>Battery_capacity</t>
+  </si>
+  <si>
+    <t>Electric_consumption_NEFZ</t>
+  </si>
+  <si>
+    <t>Fuel_consumption_NEFZ</t>
+  </si>
+  <si>
+    <t>Electric_consumption_Artemis</t>
+  </si>
+  <si>
+    <t>Fuel_consumption_Artemis</t>
+  </si>
+  <si>
+    <t>Maximum_SOC</t>
+  </si>
+  <si>
+    <t>Minimum_SOC</t>
+  </si>
+  <si>
+    <t>Rated_power_of_charging_column</t>
+  </si>
+  <si>
+    <t>Is_BEV?</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -560,23 +560,23 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -584,7 +584,7 @@
     </row>
     <row r="5" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="3"/>
@@ -622,7 +622,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" s="9">
         <v>50</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B9" s="10">
         <v>20</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B10" s="10">
         <v>1</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B11" s="10">
         <v>15</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B12" s="10">
         <v>1</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B13" s="11">
         <v>0.97</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B14" s="11">
         <v>0.03</v>
@@ -729,7 +729,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B15" s="8">
         <v>11</v>
@@ -740,13 +740,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B16" s="8">
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Removed fixme in gridModelBuilder
</commit_message>
<xml_diff>
--- a/inputData/VencoPy_scalarInputSES.xlsx
+++ b/inputData/VencoPy_scalarInputSES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vencopy_repo\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACF87F7-9851-4232-A95B-C8C9D23783C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DC4267-0FFE-4DF1-A5AC-C39E6D68C3D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added probablitites for charging station
</commit_message>
<xml_diff>
--- a/inputData/VencoPy_scalarInputSES.xlsx
+++ b/inputData/VencoPy_scalarInputSES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vencopy_repo\inputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\vencopy_internal\vencopy\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DC4267-0FFE-4DF1-A5AC-C39E6D68C3D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EB14D1-07D1-42E4-9238-002C81DDB77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs of Model" sheetId="1" r:id="rId1"/>
@@ -207,8 +207,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -547,23 +547,23 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>11</v>
       </c>
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -579,10 +579,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
@@ -600,7 +600,7 @@
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
@@ -620,7 +620,7 @@
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -637,7 +637,7 @@
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -654,7 +654,7 @@
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -671,7 +671,7 @@
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -683,7 +683,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
@@ -694,7 +694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -705,7 +705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
@@ -716,7 +716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -727,18 +727,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="8">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
@@ -752,21 +752,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" s="12"/>
       <c r="E20" s="13"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" s="12"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" s="12"/>
       <c r="E22" s="14"/>
     </row>

</xml_diff>